<commit_message>
adding modied scenario file
</commit_message>
<xml_diff>
--- a/Test Scenario/TestScenario_nopCommerce.xlsx
+++ b/Test Scenario/TestScenario_nopCommerce.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manual testing learning\Noo Commerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\manual testing\nopCommerce-Manual-Testing-Project\Test Scenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246978C5-284E-4B09-9526-FAEB088591B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B333E98C-F9D8-4CDA-AFA9-9BD95D740547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7D605DF9-02AC-4495-9BA3-101519E2FE43}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases nopCommerce" sheetId="1" r:id="rId1"/>
+    <sheet name="TestScenario nopCommerce" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB343EA-6448-4096-AC05-E98FB9E1F5C3}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.3"/>
@@ -812,7 +812,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="28">
-        <v>41697</v>
+        <v>45349</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="25"/>

</xml_diff>